<commit_message>
faltam 3DS ETIM e 2DS MODULAR
</commit_message>
<xml_diff>
--- a/PAMI-A.xlsx
+++ b/PAMI-A.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\professor\Desktop\AF AVALIACAO FINAL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79808DF1-8556-412B-8B38-CABD55F0D24F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{681D4665-5086-44D2-9338-648112670D45}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7515" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ALUNOS" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="63">
   <si>
     <t>RM</t>
   </si>
@@ -207,6 +207,9 @@
   </si>
   <si>
     <t xml:space="preserve">luiz gustavo </t>
+  </si>
+  <si>
+    <t>M3</t>
   </si>
 </sst>
 </file>
@@ -615,14 +618,14 @@
   <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="H2" sqref="H2:H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.1796875" customWidth="1"/>
-    <col min="2" max="2" width="43.90625" customWidth="1"/>
-    <col min="3" max="11" width="9.1796875" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" customWidth="1"/>
+    <col min="2" max="2" width="43.85546875" customWidth="1"/>
+    <col min="3" max="11" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -647,7 +650,9 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1"/>
+      <c r="H1" s="1" t="s">
+        <v>62</v>
+      </c>
       <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
@@ -1312,11 +1317,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.453125" customWidth="1"/>
-    <col min="2" max="3" width="11.81640625" customWidth="1"/>
-    <col min="4" max="4" width="9.1796875" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" customWidth="1"/>
+    <col min="2" max="3" width="11.85546875" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">

</xml_diff>